<commit_message>
[Laravel] Modelos y Migraciones - Creado y actualizado modelos y migraciones
</commit_message>
<xml_diff>
--- a/api/BD/DB - Progreso partes.xlsx
+++ b/api/BD/DB - Progreso partes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PROGRAMACION\Projecte-final-2DAM\api\BD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06670213-68D9-4DED-B76F-0443F8C9936F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E0CC23E-DAC0-445A-AEE8-47C2A64D56AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11664" yWindow="3432" windowWidth="11376" windowHeight="8928" xr2:uid="{26773419-7DFE-49EB-A28A-EF38862ACEA3}"/>
+    <workbookView xWindow="16836" yWindow="540" windowWidth="11376" windowHeight="8928" xr2:uid="{26773419-7DFE-49EB-A28A-EF38862ACEA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="24">
   <si>
     <t>Migrations</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Favoritos</t>
   </si>
   <si>
-    <t>ProductosFavoritos</t>
-  </si>
-  <si>
     <t>Categorias</t>
   </si>
   <si>
@@ -63,38 +60,56 @@
     <t>ProductosEspecificos</t>
   </si>
   <si>
-    <t>ProductosCategorias</t>
-  </si>
-  <si>
     <t>Tiendas</t>
   </si>
   <si>
-    <t>TiendasCategorias</t>
-  </si>
-  <si>
-    <t>ProductosTiendas</t>
-  </si>
-  <si>
     <t>Pedidos</t>
   </si>
   <si>
-    <t>ProductosPedidos</t>
-  </si>
-  <si>
     <t>Pagos</t>
   </si>
   <si>
     <t>X</t>
   </si>
   <si>
-    <t>/</t>
+    <t>Producto_Favorito</t>
+  </si>
+  <si>
+    <t>Producto_Categoria</t>
+  </si>
+  <si>
+    <t>Tienda_Categoria</t>
+  </si>
+  <si>
+    <t>Producto_Tienda</t>
+  </si>
+  <si>
+    <t>Producto_Pedido</t>
+  </si>
+  <si>
+    <t>Rutinas</t>
+  </si>
+  <si>
+    <t>Principales</t>
+  </si>
+  <si>
+    <t>Intermedias</t>
+  </si>
+  <si>
+    <t>EXPANDIR</t>
+  </si>
+  <si>
+    <t>Suscripciones</t>
+  </si>
+  <si>
+    <t>NO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,6 +142,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -283,7 +306,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -315,6 +338,17 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -631,20 +665,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79A53F59-074D-4E17-901F-A618D928E378}">
-  <dimension ref="B2:E17"/>
+  <dimension ref="A2:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="4" width="11.5546875" style="1"/>
-    <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="2:5" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="H2" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+    </row>
+    <row r="3" spans="1:11" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
@@ -655,66 +703,130 @@
         <v>2</v>
       </c>
       <c r="E3" s="6"/>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="H3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="6"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="3"/>
+        <v>12</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="E4" s="8" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="H4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="12"/>
+      <c r="J4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+        <v>12</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="E5" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="3"/>
+      <c r="K5" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+        <v>12</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="E6" s="8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="H6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B7" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+        <v>12</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="E7" s="8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="H7" s="7"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>17</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
       <c r="E8" s="8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="H8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9" s="7" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -722,87 +834,145 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10" s="7" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="D10" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="E10" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B11" s="7" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B12" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>17</v>
-      </c>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B12" s="7"/>
+      <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B13" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="12"/>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B13" s="7"/>
+      <c r="C13" s="3"/>
       <c r="D13" s="3"/>
-      <c r="E13" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B14" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B15" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B16" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="9"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="11" t="s">
-        <v>16</v>
-      </c>
+      <c r="E13" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" s="18"/>
+    </row>
+    <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E15" s="18"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="17"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="17"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="17"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="17"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="17"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="17"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="17"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="17"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="17"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="17"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="17"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="17"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="17"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="17"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="H2:K2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
[API] BD - Actualizado BD y esquema
</commit_message>
<xml_diff>
--- a/api/BD/DB - Progreso partes.xlsx
+++ b/api/BD/DB - Progreso partes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PROGRAMACION\Projecte-final-2DAM\api\BD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E0CC23E-DAC0-445A-AEE8-47C2A64D56AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4ACF7B4-3DE9-4782-B426-D5D1DC47BF6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16836" yWindow="540" windowWidth="11376" windowHeight="8928" xr2:uid="{26773419-7DFE-49EB-A28A-EF38862ACEA3}"/>
+    <workbookView xWindow="11664" yWindow="540" windowWidth="11376" windowHeight="8928" xr2:uid="{26773419-7DFE-49EB-A28A-EF38862ACEA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="25">
   <si>
     <t>Migrations</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>NO</t>
+  </si>
+  <si>
+    <t>Horarios</t>
   </si>
 </sst>
 </file>
@@ -159,7 +162,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -302,11 +305,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -345,12 +387,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -667,8 +715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79A53F59-074D-4E17-901F-A618D928E378}">
   <dimension ref="A2:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -679,18 +727,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="H2" s="19" t="s">
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="H2" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
     </row>
     <row r="3" spans="1:11" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
@@ -851,7 +899,9 @@
         <v>12</v>
       </c>
       <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="E11" s="8" t="s">
         <v>4</v>
       </c>
@@ -865,108 +915,113 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B13" s="7"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="15" t="s">
+      <c r="B13" s="19"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="18"/>
-    </row>
-    <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="16" t="s">
+      <c r="H13" s="17"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B14" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E15" s="18"/>
+    <row r="15" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="9"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="11" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="17"/>
+      <c r="A16" s="16"/>
       <c r="B16" s="13"/>
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="17"/>
+      <c r="A17" s="16"/>
       <c r="B17" s="13"/>
       <c r="C17" s="13"/>
       <c r="D17" s="13"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="17"/>
+      <c r="A18" s="16"/>
       <c r="B18" s="13"/>
       <c r="C18" s="13"/>
       <c r="D18" s="13"/>
       <c r="E18" s="14"/>
-      <c r="F18" s="17"/>
+      <c r="F18" s="16"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="17"/>
+      <c r="A19" s="16"/>
       <c r="B19" s="13"/>
       <c r="C19" s="13"/>
       <c r="D19" s="13"/>
       <c r="E19" s="14"/>
-      <c r="F19" s="17"/>
+      <c r="F19" s="16"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="17"/>
+      <c r="A20" s="16"/>
       <c r="B20" s="13"/>
       <c r="C20" s="13"/>
       <c r="D20" s="13"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="17"/>
+      <c r="A21" s="16"/>
       <c r="B21" s="13"/>
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="17"/>
+      <c r="A22" s="16"/>
       <c r="B22" s="13"/>
       <c r="C22" s="13"/>
       <c r="D22" s="13"/>
       <c r="E22" s="14"/>
-      <c r="F22" s="17"/>
+      <c r="F22" s="16"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="17"/>
+      <c r="A23" s="16"/>
       <c r="B23" s="13"/>
       <c r="C23" s="13"/>
       <c r="D23" s="13"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="17"/>
+      <c r="A24" s="16"/>
       <c r="B24" s="13"/>
       <c r="C24" s="13"/>
       <c r="D24" s="13"/>
       <c r="E24" s="14"/>
-      <c r="F24" s="17"/>
+      <c r="F24" s="16"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="17"/>
+      <c r="A25" s="16"/>
       <c r="B25" s="13"/>
       <c r="C25" s="13"/>
       <c r="D25" s="13"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>